<commit_message>
peinture + début css
</commit_message>
<xml_diff>
--- a/Objectif.xlsx
+++ b/Objectif.xlsx
@@ -456,6 +456,9 @@
       <c r="A14" t="str">
         <v>time</v>
       </c>
+      <c r="B14" t="str">
+        <v>ok (plusieurs)</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -513,6 +516,9 @@
     <row r="22">
       <c r="A22" t="str">
         <v>Faire un formulaire</v>
+      </c>
+      <c r="B22" t="str">
+        <v>ok (1)</v>
       </c>
     </row>
     <row r="23">

</xml_diff>